<commit_message>
update the package and finished the bom
</commit_message>
<xml_diff>
--- a/data_bom.xlsx
+++ b/data_bom.xlsx
@@ -578,7 +578,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6500</v>
+        <v>6507</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6500</v>
+        <v>6507</v>
       </c>
       <c r="B3" t="n">
         <v>2</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6500</v>
+        <v>6507</v>
       </c>
       <c r="B4" t="n">
         <v>3</v>
@@ -908,7 +908,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6500</v>
+        <v>6507</v>
       </c>
       <c r="B5" t="n">
         <v>4</v>
@@ -1018,7 +1018,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6500</v>
+        <v>6507</v>
       </c>
       <c r="B6" t="n">
         <v>5</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6500</v>
+        <v>6507</v>
       </c>
       <c r="B7" t="n">
         <v>6</v>
@@ -1233,116 +1233,6 @@
         <v>0</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6500</v>
-      </c>
-      <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="n">
-        <v>21137</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>71</v>
-      </c>
-      <c r="G8" t="n">
-        <v>371</v>
-      </c>
-      <c r="H8" t="n">
-        <v>385</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" t="s">
-        <v>38</v>
-      </c>
-      <c r="M8" t="n">
-        <v>100</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="O8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>39</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>39</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" t="n">
-        <v>1059</v>
-      </c>
-      <c r="W8" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>